<commit_message>
parsing category on wakepark
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -498,194 +498,354 @@
       </c>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="4">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>Лонгборд KRYPTONICS Islander</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>532 руб.</t>
         </is>
       </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>Лонгборд LANDYACHTZ Hollowtech Stratus Red Standard Flex</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>1 103,20 руб.</t>
         </is>
       </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="4">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>Лонгборд LANDYACHTZ Hollowtech Switchblade 40 Mountain Yellow</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>1 010,80 руб.</t>
         </is>
       </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="4">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>Дека для лонгборда LANDYACHTZ Hollowtech Tomahawk Topographic</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>708,40 руб.</t>
         </is>
       </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="4">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>Лонгборд LANDYACHTZ Hollowtech Tomahawk Topographic</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>1 010,80 руб.</t>
         </is>
       </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="4">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="3" t="inlineStr">
         <is>
           <t>Лонгборд LANDYACHTZ Hollowtech Wolfshark Re-Issue</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
         <is>
           <t>1 010,80 руб.</t>
         </is>
       </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="4">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>Лонгборд LANDYACHTZ Ten Two Four Wolf</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
         <is>
           <t>870,80 руб.</t>
         </is>
       </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="13.8" customHeight="1" s="4">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="3" t="inlineStr">
         <is>
           <t>Лонгборд LANDYACHTZ Gambler</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
         <is>
           <t>882 руб.</t>
         </is>
       </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="4">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="3" t="inlineStr">
         <is>
           <t>Лонгборд LANDYACHTZ Hollowtech Cheesegrater</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
         <is>
           <t>968,80 руб.</t>
         </is>
       </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="4">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="3" t="inlineStr">
         <is>
           <t>Лонгборд LANDYACHTZ Hollowtech Sidewalker</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
         <is>
           <t>1 036 руб.</t>
         </is>
       </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="4">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="3" t="inlineStr">
         <is>
           <t>Лонгборд LANDYACHTZ Battle Axe Bengal Complete</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
         <is>
           <t>882 руб.</t>
         </is>
       </c>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="4">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="3" t="inlineStr">
         <is>
           <t>Лонгборд LANDYACHTZ Battle Axe Space Rock</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
         <is>
           <t>742 руб.</t>
         </is>
       </c>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="4">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="3" t="inlineStr">
         <is>
           <t>Лонгборд LANDYACHTZ Drop Cat 38 Illuminacion Complete</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
         <is>
           <t>882 руб.</t>
         </is>
       </c>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="4">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="3" t="inlineStr">
         <is>
           <t>Лонгборд LANDYACHTZ Drop Hammer Walnut Complete</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
         <is>
           <t>834,40 руб.</t>
         </is>
       </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="4">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="3" t="inlineStr">
         <is>
           <t>Лонгборд LANDYACHTZ Drop Hammer White Oak Complete</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
         <is>
           <t>834,40 руб.</t>
         </is>
       </c>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="4">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="3" t="inlineStr">
         <is>
           <t>Лонгборд LANDYACHTZ Evo 36 Spectrum Complete</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
         <is>
           <t>924 руб.</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>NONE</t>
         </is>
       </c>
     </row>

</xml_diff>